<commit_message>
Update 1.1 R14 & R15 VUSB sense CP2102
</commit_message>
<xml_diff>
--- a/Hardware/C3-27-epaper-touch/production/C3-27-epaper-touch-all-pos-C3.xlsx
+++ b/Hardware/C3-27-epaper-touch/production/C3-27-epaper-touch-all-pos-C3.xlsx
@@ -34,19 +34,9 @@
   <numFmts count="1">
     <numFmt formatCode="0.000000" numFmtId="100"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
-      <color rgb="FF000000"/>
-      <name val="Sans"/>
-      <vertAlign val="baseline"/>
-      <sz val="10"/>
-      <strike val="0"/>
-    </font>
-    <font>
-      <b val="1"/>
       <i val="0"/>
       <u val="none"/>
       <color rgb="FF000000"/>
@@ -86,16 +76,8 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="100" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
@@ -120,7 +102,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="12.99921875" customWidth="1"/>
+    <col min="1" max="1" style="0" width="9.142307692307693"/>
     <col min="2" max="2" style="0" width="11.570733173076924" bestFit="1" customWidth="1"/>
     <col min="3" max="3" style="0" width="13.14206730769231" bestFit="1" customWidth="1"/>
     <col min="4" max="4" style="0" width="11.999278846153848" bestFit="1" customWidth="1"/>
@@ -128,25 +110,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Mid X</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Mid Y</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Rotation</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Layer</t>
         </is>
@@ -158,13 +140,13 @@
           <t>C1</t>
         </is>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>142.59999999999999</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>-85.200000000000003</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>90</v>
       </c>
       <c r="E2" t="s">
@@ -177,13 +159,13 @@
           <t>C2</t>
         </is>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>134.51249999999999</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>-83.049999999999997</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" t="s">
@@ -196,13 +178,13 @@
           <t>C3</t>
         </is>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>151.55000000000001</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>-85</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>90</v>
       </c>
       <c r="E4" t="s">
@@ -215,13 +197,13 @@
           <t>C4</t>
         </is>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>154.75</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>-85.650000000000006</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>180</v>
       </c>
       <c r="E5" t="s">
@@ -234,13 +216,13 @@
           <t>C5</t>
         </is>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>149.09999999999999</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>-90.799999999999997</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>180</v>
       </c>
       <c r="E6" t="s">
@@ -253,13 +235,13 @@
           <t>C6</t>
         </is>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>156.09999999999999</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>-69.962500000000006</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>90</v>
       </c>
       <c r="E7" t="s">
@@ -272,13 +254,13 @@
           <t>C7</t>
         </is>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>151.09999999999999</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>-96</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>180</v>
       </c>
       <c r="E8" t="s">
@@ -291,13 +273,13 @@
           <t>C8</t>
         </is>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>149.30000000000001</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>-86.099999999999994</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <v>90</v>
       </c>
       <c r="E9" t="s">
@@ -310,13 +292,13 @@
           <t>C9</t>
         </is>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>158.40000000000001</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <v>-71</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
         <v>-90</v>
       </c>
       <c r="E10" t="s">
@@ -329,13 +311,13 @@
           <t>C10</t>
         </is>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>152.69999999999999</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>-88.5</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
         <v>180</v>
       </c>
       <c r="E11" t="s">
@@ -348,13 +330,13 @@
           <t>C11</t>
         </is>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="1">
         <v>156.58750000000001</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="1">
         <v>-88.5</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" t="s">
@@ -367,13 +349,13 @@
           <t>C12</t>
         </is>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="1">
         <v>152.625</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="1">
         <v>-99.049999999999997</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" t="s">
@@ -386,13 +368,13 @@
           <t>C13</t>
         </is>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="1">
         <v>127.7</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="1">
         <v>-112.3</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" t="s">
@@ -405,13 +387,13 @@
           <t>C14</t>
         </is>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="1">
         <v>121.98999999999999</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="1">
         <v>-113.2</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" t="s">
@@ -424,13 +406,13 @@
           <t>C15</t>
         </is>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="1">
         <v>115.79000000000001</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="1">
         <v>-115.95999999999999</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
         <v>180</v>
       </c>
       <c r="E16" t="s">
@@ -443,13 +425,13 @@
           <t>C16</t>
         </is>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="1">
         <v>157.16249999999999</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="1">
         <v>-123.27</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" t="s">
@@ -462,13 +444,13 @@
           <t>C17</t>
         </is>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="1">
         <v>129.59999999999999</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="1">
         <v>-78.799999999999997</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="1">
         <v>180</v>
       </c>
       <c r="E18" t="s">
@@ -481,13 +463,13 @@
           <t>C18</t>
         </is>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="1">
         <v>134.69999999999999</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="1">
         <v>-78.799999999999997</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" t="s">
@@ -500,13 +482,13 @@
           <t>C19</t>
         </is>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="1">
         <v>128.12</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="1">
         <v>-110.18000000000001</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="1">
         <v>180</v>
       </c>
       <c r="E20" t="s">
@@ -519,13 +501,13 @@
           <t>C20</t>
         </is>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="1">
         <v>123.34999999999999</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="1">
         <v>-80.260000000000005</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="1">
         <v>-90</v>
       </c>
       <c r="E21" t="s">
@@ -538,14 +520,14 @@
           <t>C21</t>
         </is>
       </c>
-      <c r="B22" s="3">
-        <v>123.34999999999999</v>
-      </c>
-      <c r="C22" s="3">
-        <v>-88.915000000000006</v>
-      </c>
-      <c r="D22" s="3">
-        <v>90</v>
+      <c r="B22" s="1">
+        <v>126.43000000000001</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-88.609999999999999</v>
+      </c>
+      <c r="D22" s="1">
+        <v>180</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
@@ -557,13 +539,13 @@
           <t>D1</t>
         </is>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="1">
         <v>154.15000000000001</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="1">
         <v>-90.849999999999994</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="1">
         <v>180</v>
       </c>
       <c r="E23" t="s">
@@ -576,13 +558,13 @@
           <t>D2</t>
         </is>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="1">
         <v>156.55000000000001</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="1">
         <v>-93.950000000000003</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="1">
         <v>180</v>
       </c>
       <c r="E24" t="s">
@@ -595,13 +577,13 @@
           <t>D3</t>
         </is>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="1">
         <v>151.65000000000001</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="1">
         <v>-93.450000000000003</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="1">
         <v>0</v>
       </c>
       <c r="E25" t="s">
@@ -614,13 +596,13 @@
           <t>D4</t>
         </is>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="1">
         <v>137.47150099999999</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="1">
         <v>-72.370000000000005</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="1">
         <v>90</v>
       </c>
       <c r="E26" t="s">
@@ -633,13 +615,13 @@
           <t>D5</t>
         </is>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="1">
         <v>117.48</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="1">
         <v>-108.95999999999999</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="1">
         <v>-90</v>
       </c>
       <c r="E27" t="s">
@@ -652,13 +634,13 @@
           <t>J1</t>
         </is>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="1">
         <v>146.34999999999999</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="1">
         <v>-77.700000000000003</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="1">
         <v>180</v>
       </c>
       <c r="E28" t="s">
@@ -671,13 +653,13 @@
           <t>J2</t>
         </is>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="1">
         <v>124.8</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="1">
         <v>-120.75</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="1">
         <v>0</v>
       </c>
       <c r="E29" t="s">
@@ -690,13 +672,13 @@
           <t>J4</t>
         </is>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="1">
         <v>119.40000000000001</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="1">
         <v>-89</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="1">
         <v>180</v>
       </c>
       <c r="E30" t="s">
@@ -709,13 +691,13 @@
           <t>JP1</t>
         </is>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="1">
         <v>130.34999999999999</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="1">
         <v>-94.530000000000001</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" t="s">
@@ -728,13 +710,13 @@
           <t>L1</t>
         </is>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="1">
         <v>156.65000000000001</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="1">
         <v>-98.049999999999997</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="1">
         <v>-90</v>
       </c>
       <c r="E32" t="s">
@@ -747,13 +729,13 @@
           <t>Q1</t>
         </is>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="1">
         <v>138.65000000000001</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="1">
         <v>-86.5</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="1">
         <v>0</v>
       </c>
       <c r="E33" t="s">
@@ -766,13 +748,13 @@
           <t>Q2</t>
         </is>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="1">
         <v>154.65000000000001</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="1">
         <v>-119.84999999999999</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="1">
         <v>180</v>
       </c>
       <c r="E34" t="s">
@@ -785,13 +767,13 @@
           <t>Q3</t>
         </is>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="1">
         <v>149.30000000000001</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="1">
         <v>-102.23999999999999</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="1">
         <v>180</v>
       </c>
       <c r="E35" t="s">
@@ -804,13 +786,13 @@
           <t>R1</t>
         </is>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="1">
         <v>134.90000000000001</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="1">
         <v>-85.849999999999994</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="1">
         <v>180</v>
       </c>
       <c r="E36" t="s">
@@ -823,13 +805,13 @@
           <t>R2</t>
         </is>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="1">
         <v>158.155</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="1">
         <v>-120.81999999999999</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="1">
         <v>180</v>
       </c>
       <c r="E37" t="s">
@@ -842,13 +824,13 @@
           <t>R3</t>
         </is>
       </c>
-      <c r="B38" s="3">
-        <v>135.30000000000001</v>
-      </c>
-      <c r="C38" s="3">
-        <v>-89.530000000000001</v>
-      </c>
-      <c r="D38" s="3">
+      <c r="B38" s="1">
+        <v>135</v>
+      </c>
+      <c r="C38" s="1">
+        <v>-91.629999999999995</v>
+      </c>
+      <c r="D38" s="1">
         <v>0</v>
       </c>
       <c r="E38" t="s">
@@ -861,13 +843,13 @@
           <t>R4</t>
         </is>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="1">
         <v>158.91</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="1">
         <v>-118.48999999999999</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="1">
         <v>-90</v>
       </c>
       <c r="E39" t="s">
@@ -880,13 +862,13 @@
           <t>R5</t>
         </is>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="1">
         <v>152.91999999999999</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="1">
         <v>-103.20999999999999</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="1">
         <v>180</v>
       </c>
       <c r="E40" t="s">
@@ -899,13 +881,13 @@
           <t>R6</t>
         </is>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="1">
         <v>117.65000000000001</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="1">
         <v>-120.75</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="1">
         <v>-90</v>
       </c>
       <c r="E41" t="s">
@@ -918,13 +900,13 @@
           <t>R7</t>
         </is>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="1">
         <v>127.5</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="1">
         <v>-114.09999999999999</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="1">
         <v>0</v>
       </c>
       <c r="E42" t="s">
@@ -937,13 +919,13 @@
           <t>R8</t>
         </is>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="1">
         <v>155</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="1">
         <v>-115.84999999999999</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="1">
         <v>90</v>
       </c>
       <c r="E43" t="s">
@@ -956,13 +938,13 @@
           <t>R9</t>
         </is>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="1">
         <v>121.02500000000001</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="1">
         <v>-95.819999999999993</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="1">
         <v>0</v>
       </c>
       <c r="E44" t="s">
@@ -975,13 +957,13 @@
           <t>R10</t>
         </is>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="1">
         <v>118.825</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="1">
         <v>-94.200000000000003</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="1">
         <v>180</v>
       </c>
       <c r="E45" t="s">
@@ -994,14 +976,14 @@
           <t>R11</t>
         </is>
       </c>
-      <c r="B46" s="3">
-        <v>128.94999999999999</v>
-      </c>
-      <c r="C46" s="3">
-        <v>-90.549999999999997</v>
-      </c>
-      <c r="D46" s="3">
-        <v>0</v>
+      <c r="B46" s="1">
+        <v>125.70999999999999</v>
+      </c>
+      <c r="C46" s="1">
+        <v>-91.629999999999995</v>
+      </c>
+      <c r="D46" s="1">
+        <v>180</v>
       </c>
       <c r="E46" t="s">
         <v>1</v>
@@ -1013,13 +995,13 @@
           <t>R12</t>
         </is>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="1">
         <v>120.01000000000001</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="1">
         <v>-98.180000000000007</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="1">
         <v>-90</v>
       </c>
       <c r="E47" t="s">
@@ -1032,13 +1014,13 @@
           <t>R13</t>
         </is>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="1">
         <v>129.50999999999999</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="1">
         <v>-107.3</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="1">
         <v>90</v>
       </c>
       <c r="E48" t="s">
@@ -1051,13 +1033,13 @@
           <t>R14</t>
         </is>
       </c>
-      <c r="B49" s="3">
-        <v>129.47999999999999</v>
-      </c>
-      <c r="C49" s="3">
-        <v>-105.22</v>
-      </c>
-      <c r="D49" s="3">
+      <c r="B49" s="1">
+        <v>130.27000000000001</v>
+      </c>
+      <c r="C49" s="1">
+        <v>-104.94</v>
+      </c>
+      <c r="D49" s="1">
         <v>0</v>
       </c>
       <c r="E49" t="s">
@@ -1070,14 +1052,14 @@
           <t>R15</t>
         </is>
       </c>
-      <c r="B50" s="3">
-        <v>129.25999999999999</v>
-      </c>
-      <c r="C50" s="3">
-        <v>-103.92</v>
-      </c>
-      <c r="D50" s="3">
-        <v>-90</v>
+      <c r="B50" s="1">
+        <v>130.27000000000001</v>
+      </c>
+      <c r="C50" s="1">
+        <v>-103.43000000000001</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
       </c>
       <c r="E50" t="s">
         <v>1</v>
@@ -1089,13 +1071,13 @@
           <t>U1</t>
         </is>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="1">
         <v>142.51400000000001</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="1">
         <v>-114.75</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="1">
         <v>180</v>
       </c>
       <c r="E51" t="s">
@@ -1108,13 +1090,13 @@
           <t>U2</t>
         </is>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="1">
         <v>125.15000000000001</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="1">
         <v>-105.72499999999999</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="1">
         <v>90</v>
       </c>
       <c r="E52" t="s">
@@ -1127,13 +1109,13 @@
           <t>U3</t>
         </is>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="1">
         <v>118.05</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="1">
         <v>-113.19</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="1">
         <v>0</v>
       </c>
       <c r="E53" t="s">
@@ -1146,13 +1128,13 @@
           <t>U4</t>
         </is>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="1">
         <v>128.66</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="1">
         <v>-84.989999999999995</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="1">
         <v>0</v>
       </c>
       <c r="E54" t="s">
@@ -1165,13 +1147,13 @@
           <t>Y1</t>
         </is>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="1">
         <v>123.34999999999999</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="1">
         <v>-84.159999999999997</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="1">
         <v>90</v>
       </c>
       <c r="E55" t="s">

</xml_diff>

<commit_message>
C3 1.1 remove C13 does not seem to be necessary (near CP2102)
</commit_message>
<xml_diff>
--- a/Hardware/C3-27-epaper-touch/production/C3-27-epaper-touch-all-pos-C3.xlsx
+++ b/Hardware/C3-27-epaper-touch/production/C3-27-epaper-touch-all-pos-C3.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
-  <si>
-    <t>Designator</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
   <si>
     <t>top</t>
   </si>
@@ -94,10 +91,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1:E1"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -106,12 +103,14 @@
     <col min="2" max="2" style="0" width="11.570733173076924" bestFit="1" customWidth="1"/>
     <col min="3" max="3" style="0" width="13.14206730769231" bestFit="1" customWidth="1"/>
     <col min="4" max="4" style="0" width="11.999278846153848" bestFit="1" customWidth="1"/>
-    <col min="5" max="256" style="0" width="9.142307692307693"/>
+    <col min="5" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Designator</t>
+        </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
@@ -150,7 +149,7 @@
         <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -169,7 +168,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -188,7 +187,7 @@
         <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -207,7 +206,7 @@
         <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -226,7 +225,7 @@
         <v>180</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -245,7 +244,7 @@
         <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -264,7 +263,7 @@
         <v>180</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -283,7 +282,7 @@
         <v>90</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -302,7 +301,7 @@
         <v>-90</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -321,7 +320,7 @@
         <v>180</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -340,7 +339,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -359,805 +358,786 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C13</t>
+          <t>C14</t>
         </is>
       </c>
       <c r="B14" s="1">
-        <v>127.7</v>
+        <v>121.98999999999999</v>
       </c>
       <c r="C14" s="1">
-        <v>-112.3</v>
+        <v>-113.2</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C14</t>
+          <t>C15</t>
         </is>
       </c>
       <c r="B15" s="1">
-        <v>121.98999999999999</v>
+        <v>115.79000000000001</v>
       </c>
       <c r="C15" s="1">
-        <v>-113.2</v>
+        <v>-115.95999999999999</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C15</t>
+          <t>C16</t>
         </is>
       </c>
       <c r="B16" s="1">
-        <v>115.79000000000001</v>
+        <v>157.16249999999999</v>
       </c>
       <c r="C16" s="1">
-        <v>-115.95999999999999</v>
+        <v>-123.27</v>
       </c>
       <c r="D16" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C16</t>
+          <t>C17</t>
         </is>
       </c>
       <c r="B17" s="1">
-        <v>157.16249999999999</v>
+        <v>129.59999999999999</v>
       </c>
       <c r="C17" s="1">
-        <v>-123.27</v>
+        <v>-78.799999999999997</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C17</t>
+          <t>C18</t>
         </is>
       </c>
       <c r="B18" s="1">
-        <v>129.59999999999999</v>
+        <v>134.69999999999999</v>
       </c>
       <c r="C18" s="1">
         <v>-78.799999999999997</v>
       </c>
       <c r="D18" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C18</t>
+          <t>C19</t>
         </is>
       </c>
       <c r="B19" s="1">
-        <v>134.69999999999999</v>
+        <v>128.12</v>
       </c>
       <c r="C19" s="1">
-        <v>-78.799999999999997</v>
+        <v>-110.18000000000001</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C19</t>
+          <t>C20</t>
         </is>
       </c>
       <c r="B20" s="1">
-        <v>128.12</v>
+        <v>123.34999999999999</v>
       </c>
       <c r="C20" s="1">
-        <v>-110.18000000000001</v>
+        <v>-80.260000000000005</v>
       </c>
       <c r="D20" s="1">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C20</t>
+          <t>C21</t>
         </is>
       </c>
       <c r="B21" s="1">
-        <v>123.34999999999999</v>
+        <v>126.43000000000001</v>
       </c>
       <c r="C21" s="1">
-        <v>-80.260000000000005</v>
+        <v>-88.609999999999999</v>
       </c>
       <c r="D21" s="1">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C21</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="B22" s="1">
-        <v>126.43000000000001</v>
+        <v>154.15000000000001</v>
       </c>
       <c r="C22" s="1">
-        <v>-88.609999999999999</v>
+        <v>-90.849999999999994</v>
       </c>
       <c r="D22" s="1">
         <v>180</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>D2</t>
         </is>
       </c>
       <c r="B23" s="1">
-        <v>154.15000000000001</v>
+        <v>156.55000000000001</v>
       </c>
       <c r="C23" s="1">
-        <v>-90.849999999999994</v>
+        <v>-93.950000000000003</v>
       </c>
       <c r="D23" s="1">
         <v>180</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>D3</t>
         </is>
       </c>
       <c r="B24" s="1">
-        <v>156.55000000000001</v>
+        <v>151.65000000000001</v>
       </c>
       <c r="C24" s="1">
-        <v>-93.950000000000003</v>
+        <v>-93.450000000000003</v>
       </c>
       <c r="D24" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="inlineStr">
         <is>
-          <t>D3</t>
+          <t>D4</t>
         </is>
       </c>
       <c r="B25" s="1">
-        <v>151.65000000000001</v>
+        <v>137.47150099999999</v>
       </c>
       <c r="C25" s="1">
-        <v>-93.450000000000003</v>
+        <v>-72.370000000000005</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D4</t>
+          <t>D5</t>
         </is>
       </c>
       <c r="B26" s="1">
-        <v>137.47150099999999</v>
+        <v>117.48</v>
       </c>
       <c r="C26" s="1">
-        <v>-72.370000000000005</v>
+        <v>-108.95999999999999</v>
       </c>
       <c r="D26" s="1">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="inlineStr">
         <is>
-          <t>D5</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B27" s="1">
-        <v>117.48</v>
+        <v>146.34999999999999</v>
       </c>
       <c r="C27" s="1">
-        <v>-108.95999999999999</v>
+        <v>-77.700000000000003</v>
       </c>
       <c r="D27" s="1">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>J2</t>
         </is>
       </c>
       <c r="B28" s="1">
-        <v>146.34999999999999</v>
+        <v>124.8</v>
       </c>
       <c r="C28" s="1">
-        <v>-77.700000000000003</v>
+        <v>-120.75</v>
       </c>
       <c r="D28" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="inlineStr">
         <is>
-          <t>J2</t>
+          <t>J4</t>
         </is>
       </c>
       <c r="B29" s="1">
-        <v>124.8</v>
+        <v>119.40000000000001</v>
       </c>
       <c r="C29" s="1">
-        <v>-120.75</v>
+        <v>-89</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="inlineStr">
         <is>
-          <t>J4</t>
+          <t>JP1</t>
         </is>
       </c>
       <c r="B30" s="1">
-        <v>119.40000000000001</v>
+        <v>130.34999999999999</v>
       </c>
       <c r="C30" s="1">
-        <v>-89</v>
+        <v>-94.530000000000001</v>
       </c>
       <c r="D30" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="inlineStr">
         <is>
-          <t>JP1</t>
+          <t>L1</t>
         </is>
       </c>
       <c r="B31" s="1">
-        <v>130.34999999999999</v>
+        <v>156.65000000000001</v>
       </c>
       <c r="C31" s="1">
-        <v>-94.530000000000001</v>
+        <v>-98.049999999999997</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>Q1</t>
         </is>
       </c>
       <c r="B32" s="1">
-        <v>156.65000000000001</v>
+        <v>138.65000000000001</v>
       </c>
       <c r="C32" s="1">
-        <v>-98.049999999999997</v>
+        <v>-86.5</v>
       </c>
       <c r="D32" s="1">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>Q2</t>
         </is>
       </c>
       <c r="B33" s="1">
-        <v>138.65000000000001</v>
+        <v>154.65000000000001</v>
       </c>
       <c r="C33" s="1">
-        <v>-86.5</v>
+        <v>-119.84999999999999</v>
       </c>
       <c r="D33" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>Q3</t>
         </is>
       </c>
       <c r="B34" s="1">
-        <v>154.65000000000001</v>
+        <v>149.30000000000001</v>
       </c>
       <c r="C34" s="1">
-        <v>-119.84999999999999</v>
+        <v>-102.23999999999999</v>
       </c>
       <c r="D34" s="1">
         <v>180</v>
       </c>
       <c r="E34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Q3</t>
+          <t>R1</t>
         </is>
       </c>
       <c r="B35" s="1">
-        <v>149.30000000000001</v>
+        <v>134.90000000000001</v>
       </c>
       <c r="C35" s="1">
-        <v>-102.23999999999999</v>
+        <v>-85.849999999999994</v>
       </c>
       <c r="D35" s="1">
         <v>180</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>R2</t>
         </is>
       </c>
       <c r="B36" s="1">
-        <v>134.90000000000001</v>
+        <v>158.155</v>
       </c>
       <c r="C36" s="1">
-        <v>-85.849999999999994</v>
+        <v>-120.81999999999999</v>
       </c>
       <c r="D36" s="1">
         <v>180</v>
       </c>
       <c r="E36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="B37" s="1">
-        <v>158.155</v>
+        <v>135</v>
       </c>
       <c r="C37" s="1">
-        <v>-120.81999999999999</v>
+        <v>-91.629999999999995</v>
       </c>
       <c r="D37" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R4</t>
         </is>
       </c>
       <c r="B38" s="1">
-        <v>135</v>
+        <v>158.91</v>
       </c>
       <c r="C38" s="1">
-        <v>-91.629999999999995</v>
+        <v>-118.48999999999999</v>
       </c>
       <c r="D38" s="1">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="inlineStr">
         <is>
-          <t>R4</t>
+          <t>R5</t>
         </is>
       </c>
       <c r="B39" s="1">
-        <v>158.91</v>
+        <v>152.91999999999999</v>
       </c>
       <c r="C39" s="1">
-        <v>-118.48999999999999</v>
+        <v>-103.20999999999999</v>
       </c>
       <c r="D39" s="1">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="inlineStr">
         <is>
-          <t>R5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="B40" s="1">
-        <v>152.91999999999999</v>
+        <v>117.65000000000001</v>
       </c>
       <c r="C40" s="1">
-        <v>-103.20999999999999</v>
+        <v>-120.75</v>
       </c>
       <c r="D40" s="1">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R7</t>
         </is>
       </c>
       <c r="B41" s="1">
-        <v>117.65000000000001</v>
+        <v>127.5</v>
       </c>
       <c r="C41" s="1">
-        <v>-120.75</v>
+        <v>-114.09999999999999</v>
       </c>
       <c r="D41" s="1">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="inlineStr">
         <is>
-          <t>R7</t>
+          <t>R8</t>
         </is>
       </c>
       <c r="B42" s="1">
-        <v>127.5</v>
+        <v>155</v>
       </c>
       <c r="C42" s="1">
-        <v>-114.09999999999999</v>
+        <v>-115.84999999999999</v>
       </c>
       <c r="D42" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="inlineStr">
         <is>
-          <t>R8</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="B43" s="1">
-        <v>155</v>
+        <v>121.02500000000001</v>
       </c>
       <c r="C43" s="1">
-        <v>-115.84999999999999</v>
+        <v>-95.819999999999993</v>
       </c>
       <c r="D43" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="B44" s="1">
-        <v>121.02500000000001</v>
+        <v>118.825</v>
       </c>
       <c r="C44" s="1">
-        <v>-95.819999999999993</v>
+        <v>-94.200000000000003</v>
       </c>
       <c r="D44" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R11</t>
         </is>
       </c>
       <c r="B45" s="1">
-        <v>118.825</v>
+        <v>125.70999999999999</v>
       </c>
       <c r="C45" s="1">
-        <v>-94.200000000000003</v>
+        <v>-91.629999999999995</v>
       </c>
       <c r="D45" s="1">
         <v>180</v>
       </c>
       <c r="E45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R11</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="B46" s="1">
-        <v>125.70999999999999</v>
+        <v>120.01000000000001</v>
       </c>
       <c r="C46" s="1">
-        <v>-91.629999999999995</v>
+        <v>-98.180000000000007</v>
       </c>
       <c r="D46" s="1">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R13</t>
         </is>
       </c>
       <c r="B47" s="1">
-        <v>120.01000000000001</v>
+        <v>129.50999999999999</v>
       </c>
       <c r="C47" s="1">
-        <v>-98.180000000000007</v>
+        <v>-107.3</v>
       </c>
       <c r="D47" s="1">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="inlineStr">
         <is>
-          <t>R13</t>
+          <t>R14</t>
         </is>
       </c>
       <c r="B48" s="1">
-        <v>129.50999999999999</v>
+        <v>130.27000000000001</v>
       </c>
       <c r="C48" s="1">
-        <v>-107.3</v>
+        <v>-104.94</v>
       </c>
       <c r="D48" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="inlineStr">
         <is>
-          <t>R14</t>
+          <t>R15</t>
         </is>
       </c>
       <c r="B49" s="1">
         <v>130.27000000000001</v>
       </c>
       <c r="C49" s="1">
-        <v>-104.94</v>
+        <v>-103.43000000000001</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="inlineStr">
         <is>
-          <t>R15</t>
+          <t>U1</t>
         </is>
       </c>
       <c r="B50" s="1">
-        <v>130.27000000000001</v>
+        <v>142.51400000000001</v>
       </c>
       <c r="C50" s="1">
-        <v>-103.43000000000001</v>
+        <v>-114.75</v>
       </c>
       <c r="D50" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="inlineStr">
         <is>
-          <t>U1</t>
+          <t>U2</t>
         </is>
       </c>
       <c r="B51" s="1">
-        <v>142.51400000000001</v>
+        <v>125.15000000000001</v>
       </c>
       <c r="C51" s="1">
-        <v>-114.75</v>
+        <v>-105.72499999999999</v>
       </c>
       <c r="D51" s="1">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="inlineStr">
         <is>
-          <t>U2</t>
+          <t>U3</t>
         </is>
       </c>
       <c r="B52" s="1">
-        <v>125.15000000000001</v>
+        <v>118.05</v>
       </c>
       <c r="C52" s="1">
-        <v>-105.72499999999999</v>
+        <v>-113.19</v>
       </c>
       <c r="D52" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="inlineStr">
         <is>
-          <t>U3</t>
+          <t>U4</t>
         </is>
       </c>
       <c r="B53" s="1">
-        <v>118.05</v>
+        <v>128.66</v>
       </c>
       <c r="C53" s="1">
-        <v>-113.19</v>
+        <v>-84.989999999999995</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="inlineStr">
         <is>
-          <t>U4</t>
+          <t>Y1</t>
         </is>
       </c>
       <c r="B54" s="1">
-        <v>128.66</v>
+        <v>123.34999999999999</v>
       </c>
       <c r="C54" s="1">
-        <v>-84.989999999999995</v>
+        <v>-84.159999999999997</v>
       </c>
       <c r="D54" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E54" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Y1</t>
-        </is>
-      </c>
-      <c r="B55" s="1">
-        <v>123.34999999999999</v>
-      </c>
-      <c r="C55" s="1">
-        <v>-84.159999999999997</v>
-      </c>
-      <c r="D55" s="1">
-        <v>90</v>
-      </c>
-      <c r="E55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "C3 1.1 remove C13 does not seem to be necessary (near CP2102)"
This reverts commit e9bbdf2bfd8dbd0aba68dd1d7c9680fb7645ba6f.
</commit_message>
<xml_diff>
--- a/Hardware/C3-27-epaper-touch/production/C3-27-epaper-touch-all-pos-C3.xlsx
+++ b/Hardware/C3-27-epaper-touch/production/C3-27-epaper-touch-all-pos-C3.xlsx
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
+  <si>
+    <t>Designator</t>
+  </si>
   <si>
     <t>top</t>
   </si>
@@ -91,10 +94,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -103,14 +106,12 @@
     <col min="2" max="2" style="0" width="11.570733173076924" bestFit="1" customWidth="1"/>
     <col min="3" max="3" style="0" width="13.14206730769231" bestFit="1" customWidth="1"/>
     <col min="4" max="4" style="0" width="11.999278846153848" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" style="0" width="9.142307692307693"/>
+    <col min="5" max="256" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Designator</t>
-        </is>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
@@ -149,7 +150,7 @@
         <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -168,7 +169,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -187,7 +188,7 @@
         <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -206,7 +207,7 @@
         <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -225,7 +226,7 @@
         <v>180</v>
       </c>
       <c r="E6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -244,7 +245,7 @@
         <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -263,7 +264,7 @@
         <v>180</v>
       </c>
       <c r="E8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -282,7 +283,7 @@
         <v>90</v>
       </c>
       <c r="E9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -301,7 +302,7 @@
         <v>-90</v>
       </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -320,7 +321,7 @@
         <v>180</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -339,7 +340,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -358,786 +359,805 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C14</t>
+          <t>C13</t>
         </is>
       </c>
       <c r="B14" s="1">
-        <v>121.98999999999999</v>
+        <v>127.7</v>
       </c>
       <c r="C14" s="1">
-        <v>-113.2</v>
+        <v>-112.3</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C15</t>
+          <t>C14</t>
         </is>
       </c>
       <c r="B15" s="1">
-        <v>115.79000000000001</v>
+        <v>121.98999999999999</v>
       </c>
       <c r="C15" s="1">
-        <v>-115.95999999999999</v>
+        <v>-113.2</v>
       </c>
       <c r="D15" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C16</t>
+          <t>C15</t>
         </is>
       </c>
       <c r="B16" s="1">
-        <v>157.16249999999999</v>
+        <v>115.79000000000001</v>
       </c>
       <c r="C16" s="1">
-        <v>-123.27</v>
+        <v>-115.95999999999999</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C17</t>
+          <t>C16</t>
         </is>
       </c>
       <c r="B17" s="1">
-        <v>129.59999999999999</v>
+        <v>157.16249999999999</v>
       </c>
       <c r="C17" s="1">
-        <v>-78.799999999999997</v>
+        <v>-123.27</v>
       </c>
       <c r="D17" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C18</t>
+          <t>C17</t>
         </is>
       </c>
       <c r="B18" s="1">
-        <v>134.69999999999999</v>
+        <v>129.59999999999999</v>
       </c>
       <c r="C18" s="1">
         <v>-78.799999999999997</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C19</t>
+          <t>C18</t>
         </is>
       </c>
       <c r="B19" s="1">
-        <v>128.12</v>
+        <v>134.69999999999999</v>
       </c>
       <c r="C19" s="1">
-        <v>-110.18000000000001</v>
+        <v>-78.799999999999997</v>
       </c>
       <c r="D19" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C20</t>
+          <t>C19</t>
         </is>
       </c>
       <c r="B20" s="1">
-        <v>123.34999999999999</v>
+        <v>128.12</v>
       </c>
       <c r="C20" s="1">
-        <v>-80.260000000000005</v>
+        <v>-110.18000000000001</v>
       </c>
       <c r="D20" s="1">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C21</t>
+          <t>C20</t>
         </is>
       </c>
       <c r="B21" s="1">
-        <v>126.43000000000001</v>
+        <v>123.34999999999999</v>
       </c>
       <c r="C21" s="1">
-        <v>-88.609999999999999</v>
+        <v>-80.260000000000005</v>
       </c>
       <c r="D21" s="1">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="inlineStr">
         <is>
-          <t>D1</t>
+          <t>C21</t>
         </is>
       </c>
       <c r="B22" s="1">
-        <v>154.15000000000001</v>
+        <v>126.43000000000001</v>
       </c>
       <c r="C22" s="1">
-        <v>-90.849999999999994</v>
+        <v>-88.609999999999999</v>
       </c>
       <c r="D22" s="1">
         <v>180</v>
       </c>
       <c r="E22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>D1</t>
         </is>
       </c>
       <c r="B23" s="1">
-        <v>156.55000000000001</v>
+        <v>154.15000000000001</v>
       </c>
       <c r="C23" s="1">
-        <v>-93.950000000000003</v>
+        <v>-90.849999999999994</v>
       </c>
       <c r="D23" s="1">
         <v>180</v>
       </c>
       <c r="E23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="inlineStr">
         <is>
-          <t>D3</t>
+          <t>D2</t>
         </is>
       </c>
       <c r="B24" s="1">
-        <v>151.65000000000001</v>
+        <v>156.55000000000001</v>
       </c>
       <c r="C24" s="1">
-        <v>-93.450000000000003</v>
+        <v>-93.950000000000003</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E24" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="inlineStr">
         <is>
-          <t>D4</t>
+          <t>D3</t>
         </is>
       </c>
       <c r="B25" s="1">
-        <v>137.47150099999999</v>
+        <v>151.65000000000001</v>
       </c>
       <c r="C25" s="1">
-        <v>-72.370000000000005</v>
+        <v>-93.450000000000003</v>
       </c>
       <c r="D25" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D5</t>
+          <t>D4</t>
         </is>
       </c>
       <c r="B26" s="1">
-        <v>117.48</v>
+        <v>137.47150099999999</v>
       </c>
       <c r="C26" s="1">
-        <v>-108.95999999999999</v>
+        <v>-72.370000000000005</v>
       </c>
       <c r="D26" s="1">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>D5</t>
         </is>
       </c>
       <c r="B27" s="1">
-        <v>146.34999999999999</v>
+        <v>117.48</v>
       </c>
       <c r="C27" s="1">
-        <v>-77.700000000000003</v>
+        <v>-108.95999999999999</v>
       </c>
       <c r="D27" s="1">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E27" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="inlineStr">
         <is>
-          <t>J2</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="B28" s="1">
-        <v>124.8</v>
+        <v>146.34999999999999</v>
       </c>
       <c r="C28" s="1">
-        <v>-120.75</v>
+        <v>-77.700000000000003</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E28" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="inlineStr">
         <is>
-          <t>J4</t>
+          <t>J2</t>
         </is>
       </c>
       <c r="B29" s="1">
-        <v>119.40000000000001</v>
+        <v>124.8</v>
       </c>
       <c r="C29" s="1">
-        <v>-89</v>
+        <v>-120.75</v>
       </c>
       <c r="D29" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="inlineStr">
         <is>
-          <t>JP1</t>
+          <t>J4</t>
         </is>
       </c>
       <c r="B30" s="1">
-        <v>130.34999999999999</v>
+        <v>119.40000000000001</v>
       </c>
       <c r="C30" s="1">
-        <v>-94.530000000000001</v>
+        <v>-89</v>
       </c>
       <c r="D30" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E30" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="inlineStr">
         <is>
-          <t>L1</t>
+          <t>JP1</t>
         </is>
       </c>
       <c r="B31" s="1">
-        <v>156.65000000000001</v>
+        <v>130.34999999999999</v>
       </c>
       <c r="C31" s="1">
-        <v>-98.049999999999997</v>
+        <v>-94.530000000000001</v>
       </c>
       <c r="D31" s="1">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>L1</t>
         </is>
       </c>
       <c r="B32" s="1">
-        <v>138.65000000000001</v>
+        <v>156.65000000000001</v>
       </c>
       <c r="C32" s="1">
-        <v>-86.5</v>
+        <v>-98.049999999999997</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E32" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>Q1</t>
         </is>
       </c>
       <c r="B33" s="1">
-        <v>154.65000000000001</v>
+        <v>138.65000000000001</v>
       </c>
       <c r="C33" s="1">
-        <v>-119.84999999999999</v>
+        <v>-86.5</v>
       </c>
       <c r="D33" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Q3</t>
+          <t>Q2</t>
         </is>
       </c>
       <c r="B34" s="1">
-        <v>149.30000000000001</v>
+        <v>154.65000000000001</v>
       </c>
       <c r="C34" s="1">
-        <v>-102.23999999999999</v>
+        <v>-119.84999999999999</v>
       </c>
       <c r="D34" s="1">
         <v>180</v>
       </c>
       <c r="E34" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>Q3</t>
         </is>
       </c>
       <c r="B35" s="1">
-        <v>134.90000000000001</v>
+        <v>149.30000000000001</v>
       </c>
       <c r="C35" s="1">
-        <v>-85.849999999999994</v>
+        <v>-102.23999999999999</v>
       </c>
       <c r="D35" s="1">
         <v>180</v>
       </c>
       <c r="E35" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>R1</t>
         </is>
       </c>
       <c r="B36" s="1">
-        <v>158.155</v>
+        <v>134.90000000000001</v>
       </c>
       <c r="C36" s="1">
-        <v>-120.81999999999999</v>
+        <v>-85.849999999999994</v>
       </c>
       <c r="D36" s="1">
         <v>180</v>
       </c>
       <c r="E36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R2</t>
         </is>
       </c>
       <c r="B37" s="1">
-        <v>135</v>
+        <v>158.155</v>
       </c>
       <c r="C37" s="1">
-        <v>-91.629999999999995</v>
+        <v>-120.81999999999999</v>
       </c>
       <c r="D37" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E37" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="inlineStr">
         <is>
-          <t>R4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="B38" s="1">
-        <v>158.91</v>
+        <v>135</v>
       </c>
       <c r="C38" s="1">
-        <v>-118.48999999999999</v>
+        <v>-91.629999999999995</v>
       </c>
       <c r="D38" s="1">
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="inlineStr">
         <is>
-          <t>R5</t>
+          <t>R4</t>
         </is>
       </c>
       <c r="B39" s="1">
-        <v>152.91999999999999</v>
+        <v>158.91</v>
       </c>
       <c r="C39" s="1">
-        <v>-103.20999999999999</v>
+        <v>-118.48999999999999</v>
       </c>
       <c r="D39" s="1">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="E39" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R5</t>
         </is>
       </c>
       <c r="B40" s="1">
-        <v>117.65000000000001</v>
+        <v>152.91999999999999</v>
       </c>
       <c r="C40" s="1">
-        <v>-120.75</v>
+        <v>-103.20999999999999</v>
       </c>
       <c r="D40" s="1">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E40" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="inlineStr">
         <is>
-          <t>R7</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="B41" s="1">
-        <v>127.5</v>
+        <v>117.65000000000001</v>
       </c>
       <c r="C41" s="1">
-        <v>-114.09999999999999</v>
+        <v>-120.75</v>
       </c>
       <c r="D41" s="1">
-        <v>0</v>
+        <v>-90</v>
       </c>
       <c r="E41" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="inlineStr">
         <is>
-          <t>R8</t>
+          <t>R7</t>
         </is>
       </c>
       <c r="B42" s="1">
-        <v>155</v>
+        <v>127.5</v>
       </c>
       <c r="C42" s="1">
-        <v>-115.84999999999999</v>
+        <v>-114.09999999999999</v>
       </c>
       <c r="D42" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R8</t>
         </is>
       </c>
       <c r="B43" s="1">
-        <v>121.02500000000001</v>
+        <v>155</v>
       </c>
       <c r="C43" s="1">
-        <v>-95.819999999999993</v>
+        <v>-115.84999999999999</v>
       </c>
       <c r="D43" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="B44" s="1">
-        <v>118.825</v>
+        <v>121.02500000000001</v>
       </c>
       <c r="C44" s="1">
-        <v>-94.200000000000003</v>
+        <v>-95.819999999999993</v>
       </c>
       <c r="D44" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="inlineStr">
         <is>
-          <t>R11</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="B45" s="1">
-        <v>125.70999999999999</v>
+        <v>118.825</v>
       </c>
       <c r="C45" s="1">
-        <v>-91.629999999999995</v>
+        <v>-94.200000000000003</v>
       </c>
       <c r="D45" s="1">
         <v>180</v>
       </c>
       <c r="E45" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R11</t>
         </is>
       </c>
       <c r="B46" s="1">
-        <v>120.01000000000001</v>
+        <v>125.70999999999999</v>
       </c>
       <c r="C46" s="1">
-        <v>-98.180000000000007</v>
+        <v>-91.629999999999995</v>
       </c>
       <c r="D46" s="1">
-        <v>-90</v>
+        <v>180</v>
       </c>
       <c r="E46" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="inlineStr">
         <is>
-          <t>R13</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="B47" s="1">
-        <v>129.50999999999999</v>
+        <v>120.01000000000001</v>
       </c>
       <c r="C47" s="1">
-        <v>-107.3</v>
+        <v>-98.180000000000007</v>
       </c>
       <c r="D47" s="1">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="E47" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="inlineStr">
         <is>
-          <t>R14</t>
+          <t>R13</t>
         </is>
       </c>
       <c r="B48" s="1">
-        <v>130.27000000000001</v>
+        <v>129.50999999999999</v>
       </c>
       <c r="C48" s="1">
-        <v>-104.94</v>
+        <v>-107.3</v>
       </c>
       <c r="D48" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E48" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="inlineStr">
         <is>
-          <t>R15</t>
+          <t>R14</t>
         </is>
       </c>
       <c r="B49" s="1">
         <v>130.27000000000001</v>
       </c>
       <c r="C49" s="1">
-        <v>-103.43000000000001</v>
+        <v>-104.94</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="inlineStr">
         <is>
-          <t>U1</t>
+          <t>R15</t>
         </is>
       </c>
       <c r="B50" s="1">
-        <v>142.51400000000001</v>
+        <v>130.27000000000001</v>
       </c>
       <c r="C50" s="1">
-        <v>-114.75</v>
+        <v>-103.43000000000001</v>
       </c>
       <c r="D50" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="inlineStr">
         <is>
-          <t>U2</t>
+          <t>U1</t>
         </is>
       </c>
       <c r="B51" s="1">
-        <v>125.15000000000001</v>
+        <v>142.51400000000001</v>
       </c>
       <c r="C51" s="1">
-        <v>-105.72499999999999</v>
+        <v>-114.75</v>
       </c>
       <c r="D51" s="1">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E51" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="inlineStr">
         <is>
-          <t>U3</t>
+          <t>U2</t>
         </is>
       </c>
       <c r="B52" s="1">
-        <v>118.05</v>
+        <v>125.15000000000001</v>
       </c>
       <c r="C52" s="1">
-        <v>-113.19</v>
+        <v>-105.72499999999999</v>
       </c>
       <c r="D52" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E52" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="inlineStr">
         <is>
-          <t>U4</t>
+          <t>U3</t>
         </is>
       </c>
       <c r="B53" s="1">
-        <v>128.66</v>
+        <v>118.05</v>
       </c>
       <c r="C53" s="1">
-        <v>-84.989999999999995</v>
+        <v>-113.19</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="inlineStr">
         <is>
+          <t>U4</t>
+        </is>
+      </c>
+      <c r="B54" s="1">
+        <v>128.66</v>
+      </c>
+      <c r="C54" s="1">
+        <v>-84.989999999999995</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>Y1</t>
         </is>
       </c>
-      <c r="B54" s="1">
+      <c r="B55" s="1">
         <v>123.34999999999999</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C55" s="1">
         <v>-84.159999999999997</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D55" s="1">
         <v>90</v>
       </c>
-      <c r="E54" t="s">
-        <v>0</v>
+      <c r="E55" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>